<commit_message>
Added latest Q4 FY25 quarter for Nvidia
</commit_message>
<xml_diff>
--- a/data/NVDA.xlsx
+++ b/data/NVDA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tngam\projects\python\stock-kpi-plot\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38C2754A-027D-42D4-9BA3-9F363C2E3E92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{287CCF95-4DD4-41F8-9851-39A743EA9D0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4710" yWindow="13940" windowWidth="28800" windowHeight="15370" xr2:uid="{847D2414-6927-4BEE-9896-7F31C50B6E3E}"/>
+    <workbookView xWindow="8380" yWindow="10380" windowWidth="38380" windowHeight="20880" xr2:uid="{847D2414-6927-4BEE-9896-7F31C50B6E3E}"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Report Date</t>
   </si>
@@ -87,6 +87,9 @@
   </si>
   <si>
     <t>OEM &amp; Other</t>
+  </si>
+  <si>
+    <t>Q4 FY25</t>
   </si>
 </sst>
 </file>
@@ -460,10 +463,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7699876-666C-41D6-B24A-347A2FC5C849}">
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -475,9 +478,10 @@
     <col min="7" max="7" width="10.08984375" bestFit="1" customWidth="1"/>
     <col min="8" max="10" width="9.08984375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -511,8 +515,11 @@
       <c r="K1" t="s">
         <v>10</v>
       </c>
+      <c r="L1" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -546,8 +553,11 @@
       <c r="K2" s="1">
         <v>45616</v>
       </c>
+      <c r="L2" s="1">
+        <v>45714</v>
+      </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -581,8 +591,11 @@
       <c r="K3" s="2">
         <v>30771</v>
       </c>
+      <c r="L3" s="2">
+        <v>35580</v>
+      </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -616,8 +629,11 @@
       <c r="K4" s="2">
         <v>3279</v>
       </c>
+      <c r="L4" s="2">
+        <v>2544</v>
+      </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -651,8 +667,11 @@
       <c r="K5" s="2">
         <v>486</v>
       </c>
+      <c r="L5" s="2">
+        <v>511</v>
+      </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -686,8 +705,11 @@
       <c r="K6" s="2">
         <v>449</v>
       </c>
+      <c r="L6" s="2">
+        <v>570</v>
+      </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -720,6 +742,9 @@
       </c>
       <c r="K7" s="2">
         <v>97</v>
+      </c>
+      <c r="L7" s="2">
+        <v>126</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated NVDA for latest quarters
</commit_message>
<xml_diff>
--- a/data/NVDA.xlsx
+++ b/data/NVDA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tngam\projects\python\stock-kpi-plot\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{287CCF95-4DD4-41F8-9851-39A743EA9D0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9605DCA8-5C7E-456B-806A-6B3F570F3D70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8380" yWindow="10380" windowWidth="38380" windowHeight="20880" xr2:uid="{847D2414-6927-4BEE-9896-7F31C50B6E3E}"/>
+    <workbookView xWindow="1930" yWindow="12590" windowWidth="34950" windowHeight="9890" xr2:uid="{847D2414-6927-4BEE-9896-7F31C50B6E3E}"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Report Date</t>
   </si>
@@ -90,6 +90,15 @@
   </si>
   <si>
     <t>Q4 FY25</t>
+  </si>
+  <si>
+    <t>Q1 FY26</t>
+  </si>
+  <si>
+    <t>Q2 FY26</t>
+  </si>
+  <si>
+    <t>Q3 FY26</t>
   </si>
 </sst>
 </file>
@@ -463,10 +472,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7699876-666C-41D6-B24A-347A2FC5C849}">
-  <dimension ref="A1:L7"/>
+  <dimension ref="A1:O7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -478,10 +487,11 @@
     <col min="7" max="7" width="10.08984375" bestFit="1" customWidth="1"/>
     <col min="8" max="10" width="9.08984375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10.08984375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.08984375" bestFit="1" customWidth="1"/>
+    <col min="12" max="14" width="9.08984375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -518,46 +528,64 @@
       <c r="L1" t="s">
         <v>17</v>
       </c>
+      <c r="M1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O1" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1">
-        <v>44804</v>
+        <v>44773</v>
       </c>
       <c r="C2" s="1">
-        <v>44883</v>
+        <v>44864</v>
       </c>
       <c r="D2" s="1">
-        <v>44981</v>
+        <v>44955</v>
       </c>
       <c r="E2" s="1">
-        <v>45072</v>
+        <v>45046</v>
       </c>
       <c r="F2" s="1">
-        <v>45166</v>
+        <v>45137</v>
       </c>
       <c r="G2" s="1">
-        <v>45251</v>
+        <v>45228</v>
       </c>
       <c r="H2" s="1">
-        <v>45343</v>
+        <v>45319</v>
       </c>
       <c r="I2" s="1">
-        <v>45441</v>
+        <v>45410</v>
       </c>
       <c r="J2" s="1">
-        <v>45532</v>
+        <v>45501</v>
       </c>
       <c r="K2" s="1">
-        <v>45616</v>
+        <v>45592</v>
       </c>
       <c r="L2" s="1">
-        <v>45714</v>
+        <v>45683</v>
+      </c>
+      <c r="M2" s="1">
+        <v>45774</v>
+      </c>
+      <c r="N2" s="1">
+        <v>45865</v>
+      </c>
+      <c r="O2" s="1">
+        <v>45956</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -594,8 +622,17 @@
       <c r="L3" s="2">
         <v>35580</v>
       </c>
+      <c r="M3" s="2">
+        <v>39112</v>
+      </c>
+      <c r="N3" s="2">
+        <v>41096</v>
+      </c>
+      <c r="O3" s="2">
+        <v>51215</v>
+      </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -632,8 +669,17 @@
       <c r="L4" s="2">
         <v>2544</v>
       </c>
+      <c r="M4" s="2">
+        <v>3763</v>
+      </c>
+      <c r="N4" s="2">
+        <v>4287</v>
+      </c>
+      <c r="O4" s="2">
+        <v>4265</v>
+      </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -670,8 +716,17 @@
       <c r="L5" s="2">
         <v>511</v>
       </c>
+      <c r="M5" s="2">
+        <v>509</v>
+      </c>
+      <c r="N5" s="2">
+        <v>601</v>
+      </c>
+      <c r="O5" s="2">
+        <v>760</v>
+      </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -708,8 +763,17 @@
       <c r="L6" s="2">
         <v>570</v>
       </c>
+      <c r="M6" s="2">
+        <v>567</v>
+      </c>
+      <c r="N6" s="2">
+        <v>586</v>
+      </c>
+      <c r="O6" s="2">
+        <v>592</v>
+      </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -745,6 +809,15 @@
       </c>
       <c r="L7" s="2">
         <v>126</v>
+      </c>
+      <c r="M7" s="2">
+        <v>111</v>
+      </c>
+      <c r="N7" s="2">
+        <v>173</v>
+      </c>
+      <c r="O7" s="2">
+        <v>174</v>
       </c>
     </row>
   </sheetData>

</xml_diff>